<commit_message>
230116_0458 Edited settings sample file
</commit_message>
<xml_diff>
--- a/settings_form.xlsx
+++ b/settings_form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Workspace\JandiChecker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DC180B-53CA-4EEF-A513-4E90FB22D949}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F89E42-8201-4A75-B341-33F370075433}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180" xr2:uid="{11287DBB-6F95-47B7-B9EA-EF8FA5B34F62}"/>
   </bookViews>
@@ -55,7 +55,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Actual displayed name
+          <t>Wanted displayed name of each member,
+normally it's same as nickname
 (Required)</t>
         </r>
       </text>
@@ -209,7 +210,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>Members list</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -253,10 +254,6 @@
     <t>daanta-real</t>
   </si>
   <si>
-    <t>2. Scheduler settings</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Execution time rules</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -265,26 +262,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Channel ID to show the result</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>3. API Tokens</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>JDA Token value</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ChatGPT API Token value</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gogole Cloud API Token value</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>{</t>
   </si>
   <si>
@@ -351,23 +332,95 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>What you're see is example form.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Edit contents of all of yellow cells for yours,</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>change file name to "settings.xlsx",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>and just run JandiChecker. Then profit!</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">  "token_uri": "wow means World of Warcraft",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. Scheduled commit checker settings</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">What you're see is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>example form</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Fill yellow cells to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>yours</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(member infoes, API Tokens, etc.)</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. Change file name to "settings.xlsx"</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. And just run JandiChecker.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Then, profit!</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Your JDA Token value</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Your ChatGPT API Token value</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Your Gogole Cloud API Token value</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Target Discord Channel ID to send the result</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -823,14 +876,15 @@
   <dimension ref="B2:G123"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.875" customWidth="1"/>
     <col min="2" max="4" width="16.625" customWidth="1"/>
-    <col min="6" max="6" width="30.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.875" customWidth="1"/>
+    <col min="6" max="6" width="42.5" style="4" customWidth="1"/>
     <col min="7" max="7" width="132.375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
@@ -870,7 +924,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>7</v>
@@ -881,13 +935,13 @@
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
@@ -895,7 +949,7 @@
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="F6" s="7" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="G6" s="7"/>
     </row>
@@ -904,10 +958,10 @@
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="F7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
@@ -915,10 +969,10 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="F8" s="1" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
@@ -931,7 +985,7 @@
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="F10" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G10" s="7"/>
     </row>
@@ -940,10 +994,10 @@
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="F11" s="1" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
@@ -951,10 +1005,10 @@
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="F12" s="1" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
@@ -962,10 +1016,10 @@
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="F13" s="8" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
@@ -974,7 +1028,7 @@
       <c r="D14" s="3"/>
       <c r="F14" s="8"/>
       <c r="G14" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
@@ -983,7 +1037,7 @@
       <c r="D15" s="3"/>
       <c r="F15" s="8"/>
       <c r="G15" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
@@ -992,7 +1046,7 @@
       <c r="D16" s="3"/>
       <c r="F16" s="8"/>
       <c r="G16" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
@@ -1001,7 +1055,7 @@
       <c r="D17" s="3"/>
       <c r="F17" s="8"/>
       <c r="G17" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
@@ -1010,7 +1064,7 @@
       <c r="D18" s="3"/>
       <c r="F18" s="8"/>
       <c r="G18" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
@@ -1019,7 +1073,7 @@
       <c r="D19" s="3"/>
       <c r="F19" s="8"/>
       <c r="G19" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
@@ -1028,7 +1082,7 @@
       <c r="D20" s="3"/>
       <c r="F20" s="8"/>
       <c r="G20" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
@@ -1037,7 +1091,7 @@
       <c r="D21" s="3"/>
       <c r="F21" s="8"/>
       <c r="G21" s="5" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
@@ -1046,7 +1100,7 @@
       <c r="D22" s="3"/>
       <c r="F22" s="8"/>
       <c r="G22" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
@@ -1055,7 +1109,7 @@
       <c r="D23" s="3"/>
       <c r="F23" s="8"/>
       <c r="G23" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
@@ -1064,7 +1118,7 @@
       <c r="D24" s="3"/>
       <c r="F24" s="8"/>
       <c r="G24" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
@@ -1077,7 +1131,7 @@
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="F26" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.3">
@@ -1085,7 +1139,7 @@
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="F27" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.3">
@@ -1093,7 +1147,7 @@
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="F28" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.3">
@@ -1101,13 +1155,16 @@
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="F29" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
+      <c r="F30" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B31" s="3"/>

</xml_diff>

<commit_message>
230116_2231 Added props "language"
</commit_message>
<xml_diff>
--- a/settings_form.xlsx
+++ b/settings_form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Workspace\JandiChecker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F89E42-8201-4A75-B341-33F370075433}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6499DC6-4357-4B0B-97F3-98C57661005C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180" xr2:uid="{11287DBB-6F95-47B7-B9EA-EF8FA5B34F62}"/>
   </bookViews>
@@ -121,7 +121,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F7" authorId="1" shapeId="0" xr:uid="{6DB7884E-FA75-4820-B325-165FB16F832A}">
+    <comment ref="F10" authorId="1" shapeId="0" xr:uid="{6DB7884E-FA75-4820-B325-165FB16F832A}">
       <text>
         <r>
           <rPr>
@@ -135,7 +135,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G7" authorId="0" shapeId="0" xr:uid="{057E114B-7728-465D-9913-FE67D5A9CEA4}">
+    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{057E114B-7728-465D-9913-FE67D5A9CEA4}">
       <text>
         <r>
           <rPr>
@@ -149,7 +149,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="1" shapeId="0" xr:uid="{3E63FCF1-D652-469A-8093-F37251F622A1}">
+    <comment ref="F11" authorId="1" shapeId="0" xr:uid="{3E63FCF1-D652-469A-8093-F37251F622A1}">
       <text>
         <r>
           <rPr>
@@ -163,7 +163,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{F842E091-484B-4476-AE1A-5FFBFBEC3CF6}">
+    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{F842E091-484B-4476-AE1A-5FFBFBEC3CF6}">
       <text>
         <r>
           <rPr>
@@ -177,7 +177,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{20BB6126-DA36-426E-98CE-A24233ECC8B0}">
+    <comment ref="F15" authorId="0" shapeId="0" xr:uid="{20BB6126-DA36-426E-98CE-A24233ECC8B0}">
       <text>
         <r>
           <rPr>
@@ -191,7 +191,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F13" authorId="0" shapeId="0" xr:uid="{68592C10-CFA4-4E4F-BB29-725B3DD61FDE}">
+    <comment ref="F16" authorId="0" shapeId="0" xr:uid="{68592C10-CFA4-4E4F-BB29-725B3DD61FDE}">
       <text>
         <r>
           <rPr>
@@ -210,7 +210,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>Members list</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -422,6 +422,15 @@
   <si>
     <t>Target Discord Channel ID to send the result</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Language (Choose in the select box)</t>
+  </si>
+  <si>
+    <t>2. Language settings</t>
+  </si>
+  <si>
+    <t>English</t>
   </si>
 </sst>
 </file>
@@ -460,7 +469,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -491,8 +500,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -515,19 +530,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -541,7 +572,28 @@
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -876,28 +928,29 @@
   <dimension ref="B2:G123"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.875" customWidth="1"/>
-    <col min="2" max="4" width="16.625" customWidth="1"/>
-    <col min="5" max="5" width="2.875" customWidth="1"/>
-    <col min="6" max="6" width="42.5" style="4" customWidth="1"/>
-    <col min="7" max="7" width="132.375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="2.875" style="4" customWidth="1"/>
+    <col min="2" max="4" width="16.625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="2.875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="45.125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="120.375" style="6" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="F2" s="7" t="s">
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="F2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="7"/>
+      <c r="G2" s="8"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
@@ -912,749 +965,780 @@
       <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="F6" s="7" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="F6" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="F7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="F9" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="F7" s="1" t="s">
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="F10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G10" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="F8" s="1" t="s">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="F11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G11" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="F10" s="7" t="s">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="F13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="F11" s="1" t="s">
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="F14" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G14" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="F12" s="1" t="s">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="F15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G15" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="F13" s="8" t="s">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="F16" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G16" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="5" t="s">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="5" t="s">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="5" t="s">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="5" t="s">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="5" t="s">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="5" t="s">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="5" t="s">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="5" t="s">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="5" t="s">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="5" t="s">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="5" t="s">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="F26" s="4" t="s">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="F29" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="F27" s="4" t="s">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="F30" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="F28" s="4" t="s">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="F31" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="F29" s="4" t="s">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="F32" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="F30" s="4" t="s">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="F33" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B67" s="3"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B68" s="3"/>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B69" s="3"/>
-      <c r="C69" s="3"/>
-      <c r="D69" s="3"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B71" s="3"/>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B72" s="3"/>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B73" s="3"/>
-      <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B74" s="3"/>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B75" s="3"/>
-      <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B76" s="3"/>
-      <c r="C76" s="3"/>
-      <c r="D76" s="3"/>
+      <c r="B76" s="2"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B77" s="3"/>
-      <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
+      <c r="B77" s="2"/>
+      <c r="C77" s="2"/>
+      <c r="D77" s="2"/>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B78" s="3"/>
-      <c r="C78" s="3"/>
-      <c r="D78" s="3"/>
+      <c r="B78" s="2"/>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B79" s="3"/>
-      <c r="C79" s="3"/>
-      <c r="D79" s="3"/>
+      <c r="B79" s="2"/>
+      <c r="C79" s="2"/>
+      <c r="D79" s="2"/>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B80" s="3"/>
-      <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
+      <c r="B80" s="2"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B81" s="3"/>
-      <c r="C81" s="3"/>
-      <c r="D81" s="3"/>
+      <c r="B81" s="2"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B82" s="3"/>
-      <c r="C82" s="3"/>
-      <c r="D82" s="3"/>
+      <c r="B82" s="2"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B83" s="3"/>
-      <c r="C83" s="3"/>
-      <c r="D83" s="3"/>
+      <c r="B83" s="2"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B84" s="3"/>
-      <c r="C84" s="3"/>
-      <c r="D84" s="3"/>
+      <c r="B84" s="2"/>
+      <c r="C84" s="2"/>
+      <c r="D84" s="2"/>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B85" s="3"/>
-      <c r="C85" s="3"/>
-      <c r="D85" s="3"/>
+      <c r="B85" s="2"/>
+      <c r="C85" s="2"/>
+      <c r="D85" s="2"/>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B86" s="3"/>
-      <c r="C86" s="3"/>
-      <c r="D86" s="3"/>
+      <c r="B86" s="2"/>
+      <c r="C86" s="2"/>
+      <c r="D86" s="2"/>
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B87" s="3"/>
-      <c r="C87" s="3"/>
-      <c r="D87" s="3"/>
+      <c r="B87" s="2"/>
+      <c r="C87" s="2"/>
+      <c r="D87" s="2"/>
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B88" s="3"/>
-      <c r="C88" s="3"/>
-      <c r="D88" s="3"/>
+      <c r="B88" s="2"/>
+      <c r="C88" s="2"/>
+      <c r="D88" s="2"/>
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B89" s="3"/>
-      <c r="C89" s="3"/>
-      <c r="D89" s="3"/>
+      <c r="B89" s="2"/>
+      <c r="C89" s="2"/>
+      <c r="D89" s="2"/>
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B90" s="3"/>
-      <c r="C90" s="3"/>
-      <c r="D90" s="3"/>
+      <c r="B90" s="2"/>
+      <c r="C90" s="2"/>
+      <c r="D90" s="2"/>
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B91" s="3"/>
-      <c r="C91" s="3"/>
-      <c r="D91" s="3"/>
+      <c r="B91" s="2"/>
+      <c r="C91" s="2"/>
+      <c r="D91" s="2"/>
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B92" s="3"/>
-      <c r="C92" s="3"/>
-      <c r="D92" s="3"/>
+      <c r="B92" s="2"/>
+      <c r="C92" s="2"/>
+      <c r="D92" s="2"/>
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B93" s="3"/>
-      <c r="C93" s="3"/>
-      <c r="D93" s="3"/>
+      <c r="B93" s="2"/>
+      <c r="C93" s="2"/>
+      <c r="D93" s="2"/>
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B94" s="3"/>
-      <c r="C94" s="3"/>
-      <c r="D94" s="3"/>
+      <c r="B94" s="2"/>
+      <c r="C94" s="2"/>
+      <c r="D94" s="2"/>
     </row>
     <row r="95" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B95" s="3"/>
-      <c r="C95" s="3"/>
-      <c r="D95" s="3"/>
+      <c r="B95" s="2"/>
+      <c r="C95" s="2"/>
+      <c r="D95" s="2"/>
     </row>
     <row r="96" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B96" s="3"/>
-      <c r="C96" s="3"/>
-      <c r="D96" s="3"/>
+      <c r="B96" s="2"/>
+      <c r="C96" s="2"/>
+      <c r="D96" s="2"/>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B97" s="3"/>
-      <c r="C97" s="3"/>
-      <c r="D97" s="3"/>
+      <c r="B97" s="2"/>
+      <c r="C97" s="2"/>
+      <c r="D97" s="2"/>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B98" s="3"/>
-      <c r="C98" s="3"/>
-      <c r="D98" s="3"/>
+      <c r="B98" s="2"/>
+      <c r="C98" s="2"/>
+      <c r="D98" s="2"/>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B99" s="3"/>
-      <c r="C99" s="3"/>
-      <c r="D99" s="3"/>
+      <c r="B99" s="2"/>
+      <c r="C99" s="2"/>
+      <c r="D99" s="2"/>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B100" s="3"/>
-      <c r="C100" s="3"/>
-      <c r="D100" s="3"/>
+      <c r="B100" s="2"/>
+      <c r="C100" s="2"/>
+      <c r="D100" s="2"/>
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B101" s="3"/>
-      <c r="C101" s="3"/>
-      <c r="D101" s="3"/>
+      <c r="B101" s="2"/>
+      <c r="C101" s="2"/>
+      <c r="D101" s="2"/>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B102" s="3"/>
-      <c r="C102" s="3"/>
-      <c r="D102" s="3"/>
+      <c r="B102" s="2"/>
+      <c r="C102" s="2"/>
+      <c r="D102" s="2"/>
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B103" s="3"/>
-      <c r="C103" s="3"/>
-      <c r="D103" s="3"/>
+      <c r="B103" s="2"/>
+      <c r="C103" s="2"/>
+      <c r="D103" s="2"/>
     </row>
     <row r="104" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B104" s="3"/>
-      <c r="C104" s="3"/>
-      <c r="D104" s="3"/>
+      <c r="B104" s="2"/>
+      <c r="C104" s="2"/>
+      <c r="D104" s="2"/>
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B105" s="3"/>
-      <c r="C105" s="3"/>
-      <c r="D105" s="3"/>
+      <c r="B105" s="2"/>
+      <c r="C105" s="2"/>
+      <c r="D105" s="2"/>
     </row>
     <row r="106" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B106" s="3"/>
-      <c r="C106" s="3"/>
-      <c r="D106" s="3"/>
+      <c r="B106" s="2"/>
+      <c r="C106" s="2"/>
+      <c r="D106" s="2"/>
     </row>
     <row r="107" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B107" s="3"/>
-      <c r="C107" s="3"/>
-      <c r="D107" s="3"/>
+      <c r="B107" s="2"/>
+      <c r="C107" s="2"/>
+      <c r="D107" s="2"/>
     </row>
     <row r="108" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B108" s="3"/>
-      <c r="C108" s="3"/>
-      <c r="D108" s="3"/>
+      <c r="B108" s="2"/>
+      <c r="C108" s="2"/>
+      <c r="D108" s="2"/>
     </row>
     <row r="109" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B109" s="3"/>
-      <c r="C109" s="3"/>
-      <c r="D109" s="3"/>
+      <c r="B109" s="2"/>
+      <c r="C109" s="2"/>
+      <c r="D109" s="2"/>
     </row>
     <row r="110" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B110" s="3"/>
-      <c r="C110" s="3"/>
-      <c r="D110" s="3"/>
+      <c r="B110" s="2"/>
+      <c r="C110" s="2"/>
+      <c r="D110" s="2"/>
     </row>
     <row r="111" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B111" s="3"/>
-      <c r="C111" s="3"/>
-      <c r="D111" s="3"/>
+      <c r="B111" s="2"/>
+      <c r="C111" s="2"/>
+      <c r="D111" s="2"/>
     </row>
     <row r="112" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B112" s="3"/>
-      <c r="C112" s="3"/>
-      <c r="D112" s="3"/>
+      <c r="B112" s="2"/>
+      <c r="C112" s="2"/>
+      <c r="D112" s="2"/>
     </row>
     <row r="113" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B113" s="3"/>
-      <c r="C113" s="3"/>
-      <c r="D113" s="3"/>
+      <c r="B113" s="2"/>
+      <c r="C113" s="2"/>
+      <c r="D113" s="2"/>
     </row>
     <row r="114" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B114" s="3"/>
-      <c r="C114" s="3"/>
-      <c r="D114" s="3"/>
+      <c r="B114" s="2"/>
+      <c r="C114" s="2"/>
+      <c r="D114" s="2"/>
     </row>
     <row r="115" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B115" s="3"/>
-      <c r="C115" s="3"/>
-      <c r="D115" s="3"/>
+      <c r="B115" s="2"/>
+      <c r="C115" s="2"/>
+      <c r="D115" s="2"/>
     </row>
     <row r="116" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B116" s="3"/>
-      <c r="C116" s="3"/>
-      <c r="D116" s="3"/>
+      <c r="B116" s="2"/>
+      <c r="C116" s="2"/>
+      <c r="D116" s="2"/>
     </row>
     <row r="117" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B117" s="3"/>
-      <c r="C117" s="3"/>
-      <c r="D117" s="3"/>
+      <c r="B117" s="2"/>
+      <c r="C117" s="2"/>
+      <c r="D117" s="2"/>
     </row>
     <row r="118" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B118" s="3"/>
-      <c r="C118" s="3"/>
-      <c r="D118" s="3"/>
+      <c r="B118" s="2"/>
+      <c r="C118" s="2"/>
+      <c r="D118" s="2"/>
     </row>
     <row r="119" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B119" s="3"/>
-      <c r="C119" s="3"/>
-      <c r="D119" s="3"/>
+      <c r="B119" s="2"/>
+      <c r="C119" s="2"/>
+      <c r="D119" s="2"/>
     </row>
     <row r="120" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B120" s="3"/>
-      <c r="C120" s="3"/>
-      <c r="D120" s="3"/>
+      <c r="B120" s="2"/>
+      <c r="C120" s="2"/>
+      <c r="D120" s="2"/>
     </row>
     <row r="121" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B121" s="3"/>
-      <c r="C121" s="3"/>
-      <c r="D121" s="3"/>
+      <c r="B121" s="2"/>
+      <c r="C121" s="2"/>
+      <c r="D121" s="2"/>
     </row>
     <row r="122" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B122" s="3"/>
-      <c r="C122" s="3"/>
-      <c r="D122" s="3"/>
+      <c r="B122" s="2"/>
+      <c r="C122" s="2"/>
+      <c r="D122" s="2"/>
     </row>
     <row r="123" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B123" s="3"/>
-      <c r="C123" s="3"/>
-      <c r="D123" s="3"/>
+      <c r="B123" s="2"/>
+      <c r="C123" s="2"/>
+      <c r="D123" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F16:F27"/>
+    <mergeCell ref="F9:G9"/>
     <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F13:F24"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="C1:C3 C5:C1048576">
-    <cfRule type="expression" dxfId="2" priority="3">
+  <conditionalFormatting sqref="C1 C124:C1048576">
+    <cfRule type="expression" dxfId="5" priority="7">
       <formula>AND(OFFSET(C1,0,-1)&lt;&gt;"",C1="")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G4 G7:G8 G11:G24">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
+  <conditionalFormatting sqref="C2:C123">
+    <cfRule type="expression" dxfId="4" priority="6">
+      <formula>AND(OFFSET(C2,0,-1)&lt;&gt;"",C2="")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G4">
+    <cfRule type="containsBlanks" dxfId="3" priority="5">
       <formula>LEN(TRIM(G3))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>AND(OFFSET(C4,0,-1)&lt;&gt;"",C4="")</formula>
+  <conditionalFormatting sqref="G10:G11">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(G10))=0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="G14:G27">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(G14))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(G7))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G7" xr:uid="{2DC17E54-4661-4CCC-8285-0FCF3F964171}">
+      <formula1>"English,Korean,Japanese,Chinese(Simplified),Chinese(Traditional)"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
230116_2234 Updated sheet versioni to v1.8
</commit_message>
<xml_diff>
--- a/settings_form.xlsx
+++ b/settings_form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Workspace\JandiChecker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6499DC6-4357-4B0B-97F3-98C57661005C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5ACBF5F-CD7B-4A4D-8066-4A59AA573609}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180" xr2:uid="{11287DBB-6F95-47B7-B9EA-EF8FA5B34F62}"/>
   </bookViews>
@@ -236,15 +236,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>v1.7</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>BUILD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>230115_0214</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -431,6 +423,14 @@
   </si>
   <si>
     <t>English</t>
+  </si>
+  <si>
+    <t>v1.8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>230116_2233</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -572,7 +572,14 @@
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -928,7 +935,7 @@
   <dimension ref="B2:G123"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G3" sqref="G3:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -966,35 +973,35 @@
         <v>5</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
@@ -1002,7 +1009,7 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="F6" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G6" s="8"/>
     </row>
@@ -1011,10 +1018,10 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="F7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
@@ -1027,7 +1034,7 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="F9" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G9" s="8"/>
     </row>
@@ -1036,10 +1043,10 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="F10" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
@@ -1047,10 +1054,10 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="F11" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
@@ -1063,7 +1070,7 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="F13" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G13" s="8"/>
     </row>
@@ -1072,10 +1079,10 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="F14" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
@@ -1083,10 +1090,10 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="F15" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
@@ -1094,10 +1101,10 @@
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="F16" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
@@ -1106,7 +1113,7 @@
       <c r="D17" s="2"/>
       <c r="F17" s="9"/>
       <c r="G17" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
@@ -1115,7 +1122,7 @@
       <c r="D18" s="2"/>
       <c r="F18" s="9"/>
       <c r="G18" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
@@ -1124,7 +1131,7 @@
       <c r="D19" s="2"/>
       <c r="F19" s="9"/>
       <c r="G19" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
@@ -1133,7 +1140,7 @@
       <c r="D20" s="2"/>
       <c r="F20" s="9"/>
       <c r="G20" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
@@ -1142,7 +1149,7 @@
       <c r="D21" s="2"/>
       <c r="F21" s="9"/>
       <c r="G21" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
@@ -1151,7 +1158,7 @@
       <c r="D22" s="2"/>
       <c r="F22" s="9"/>
       <c r="G22" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
@@ -1160,7 +1167,7 @@
       <c r="D23" s="2"/>
       <c r="F23" s="9"/>
       <c r="G23" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
@@ -1169,7 +1176,7 @@
       <c r="D24" s="2"/>
       <c r="F24" s="9"/>
       <c r="G24" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
@@ -1178,7 +1185,7 @@
       <c r="D25" s="2"/>
       <c r="F25" s="9"/>
       <c r="G25" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.3">
@@ -1187,7 +1194,7 @@
       <c r="D26" s="2"/>
       <c r="F26" s="9"/>
       <c r="G26" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.3">
@@ -1196,7 +1203,7 @@
       <c r="D27" s="2"/>
       <c r="F27" s="9"/>
       <c r="G27" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.3">
@@ -1209,7 +1216,7 @@
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="F29" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.3">
@@ -1217,7 +1224,7 @@
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="F30" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.3">
@@ -1225,7 +1232,7 @@
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="F31" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.3">
@@ -1233,7 +1240,7 @@
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="F32" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.3">
@@ -1241,7 +1248,7 @@
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="F33" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.3">
@@ -1705,33 +1712,33 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C1 C124:C1048576">
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="6" priority="8">
       <formula>AND(OFFSET(C1,0,-1)&lt;&gt;"",C1="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C123">
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="5" priority="7">
       <formula>AND(OFFSET(C2,0,-1)&lt;&gt;"",C2="")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G4">
-    <cfRule type="containsBlanks" dxfId="3" priority="5">
-      <formula>LEN(TRIM(G3))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="G10:G11">
-    <cfRule type="containsBlanks" dxfId="2" priority="3">
+    <cfRule type="containsBlanks" dxfId="3" priority="4">
       <formula>LEN(TRIM(G10))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14:G27">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
       <formula>LEN(TRIM(G14))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(G7))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G4">
     <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(G7))=0</formula>
+      <formula>LEN(TRIM(G3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">

</xml_diff>

<commit_message>
230118_1315 Form xlsx updated
</commit_message>
<xml_diff>
--- a/settings_form.xlsx
+++ b/settings_form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Workspace\JandiChecker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5ACBF5F-CD7B-4A4D-8066-4A59AA573609}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C2E121-8711-48FD-B90B-B803E24A6BCE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180" xr2:uid="{11287DBB-6F95-47B7-B9EA-EF8FA5B34F62}"/>
   </bookViews>
@@ -425,12 +425,11 @@
     <t>English</t>
   </si>
   <si>
-    <t>v1.8</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>230116_2233</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>v1.8.1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>230117_2327</t>
   </si>
 </sst>
 </file>
@@ -934,9 +933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84E2C0E5-B93F-4F33-9852-CA2DB37EABB4}">
   <dimension ref="B2:G123"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G4"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1712,27 +1709,27 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C1 C124:C1048576">
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="6" priority="9">
       <formula>AND(OFFSET(C1,0,-1)&lt;&gt;"",C1="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C123">
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="5" priority="8">
       <formula>AND(OFFSET(C2,0,-1)&lt;&gt;"",C2="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10:G11">
-    <cfRule type="containsBlanks" dxfId="3" priority="4">
+    <cfRule type="containsBlanks" dxfId="4" priority="5">
       <formula>LEN(TRIM(G10))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14:G27">
-    <cfRule type="containsBlanks" dxfId="2" priority="3">
+    <cfRule type="containsBlanks" dxfId="3" priority="4">
       <formula>LEN(TRIM(G14))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
       <formula>LEN(TRIM(G7))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
230612_2354 Trying for fix the error of Translation Service API
</commit_message>
<xml_diff>
--- a/settings_form.xlsx
+++ b/settings_form.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20395"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20398"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Workspace\JandiChecker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A7DB10-00B6-4DD8-937D-006F274B3E03}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766C65F8-FD5F-430C-840B-85E0C7F5678E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180" xr2:uid="{11287DBB-6F95-47B7-B9EA-EF8FA5B34F62}"/>
   </bookViews>
@@ -452,7 +452,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -490,11 +490,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -509,7 +527,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -872,7 +896,7 @@
   <dimension ref="B2:G123"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5:G5"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1012,7 +1036,7 @@
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="F13" s="8"/>
+      <c r="F13" s="9"/>
       <c r="G13" s="3" t="s">
         <v>17</v>
       </c>
@@ -1021,7 +1045,7 @@
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="F14" s="8"/>
+      <c r="F14" s="9"/>
       <c r="G14" s="3" t="s">
         <v>18</v>
       </c>
@@ -1030,7 +1054,7 @@
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="F15" s="8"/>
+      <c r="F15" s="9"/>
       <c r="G15" s="3" t="s">
         <v>19</v>
       </c>
@@ -1039,7 +1063,7 @@
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
-      <c r="F16" s="8"/>
+      <c r="F16" s="9"/>
       <c r="G16" s="3" t="s">
         <v>20</v>
       </c>
@@ -1048,7 +1072,7 @@
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
-      <c r="F17" s="8"/>
+      <c r="F17" s="9"/>
       <c r="G17" s="3" t="s">
         <v>21</v>
       </c>
@@ -1057,7 +1081,7 @@
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
-      <c r="F18" s="8"/>
+      <c r="F18" s="9"/>
       <c r="G18" s="3" t="s">
         <v>22</v>
       </c>
@@ -1066,7 +1090,7 @@
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
-      <c r="F19" s="8"/>
+      <c r="F19" s="9"/>
       <c r="G19" s="3" t="s">
         <v>23</v>
       </c>
@@ -1075,7 +1099,7 @@
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
-      <c r="F20" s="8"/>
+      <c r="F20" s="9"/>
       <c r="G20" s="3" t="s">
         <v>26</v>
       </c>
@@ -1084,7 +1108,7 @@
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="F21" s="8"/>
+      <c r="F21" s="9"/>
       <c r="G21" s="3" t="s">
         <v>24</v>
       </c>
@@ -1093,7 +1117,7 @@
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-      <c r="F22" s="8"/>
+      <c r="F22" s="9"/>
       <c r="G22" s="3" t="s">
         <v>25</v>
       </c>
@@ -1102,7 +1126,7 @@
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
-      <c r="F23" s="8"/>
+      <c r="F23" s="9"/>
       <c r="G23" s="3" t="s">
         <v>10</v>
       </c>
@@ -1111,21 +1135,20 @@
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="3"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
-      <c r="F25" s="5" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="F26" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.3">
@@ -1133,7 +1156,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="F27" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.3">
@@ -1141,7 +1164,7 @@
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="F28" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.3">
@@ -1149,13 +1172,16 @@
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="F29" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
+      <c r="F30" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B31" s="2"/>
@@ -1626,34 +1652,39 @@
   <mergeCells count="5">
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F12:F23"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F12:F24"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C1 C124:C1048576">
-    <cfRule type="expression" dxfId="5" priority="9">
+    <cfRule type="expression" dxfId="5" priority="10">
       <formula>AND(OFFSET(C1,0,-1)&lt;&gt;"",C1="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C123">
-    <cfRule type="expression" dxfId="4" priority="8">
+    <cfRule type="expression" dxfId="4" priority="9">
       <formula>AND(OFFSET(C2,0,-1)&lt;&gt;"",C2="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G7">
-    <cfRule type="containsBlanks" dxfId="3" priority="5">
+    <cfRule type="containsBlanks" dxfId="3" priority="6">
       <formula>LEN(TRIM(G6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10:G23">
-    <cfRule type="containsBlanks" dxfId="2" priority="4">
+    <cfRule type="containsBlanks" dxfId="2" priority="5">
       <formula>LEN(TRIM(G10))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="containsBlanks" dxfId="1" priority="3">
+    <cfRule type="containsBlanks" dxfId="1" priority="4">
       <formula>LEN(TRIM(G3))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G24">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(G24))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">

</xml_diff>